<commit_message>
chore : update jnvtrl
</commit_message>
<xml_diff>
--- a/Doc/JNTRVL-PlotThatLine-MaresJulien.xlsx
+++ b/Doc/JNTRVL-PlotThatLine-MaresJulien.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\px50vpm\Documents\GitHub\Plot-that-line\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5DA729E-1E2C-4ECA-B525-CF9D5F3BFC67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D4B6F6A-5A22-4F13-88C9-88B5D312BB9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="Mvap2W10CJFFJsnvkGXSiMLvpngxTMJbJsIKFe7Hzjn0XDcmjGuvBC2FjUCZ/hpRpUhUrG1T4kBlDAIo3yqmSQ==" workbookSaltValue="KXjgXOcsUZI/j7UgPKltzw==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="51">
   <si>
     <t>Journal de travail</t>
   </si>
@@ -183,6 +183,21 @@
   </si>
   <si>
     <t>5mn J'ai eu un petit prbl en ouvrant mon programme le designer avait une erreur je pouvais plus le voir ou le modifier, il a juste fallu supprimer les dossier .vs, bin et obj</t>
+  </si>
+  <si>
+    <t>Création journal de travail (sur excel) et ajouts des tâches faites les semaines précédentes</t>
+  </si>
+  <si>
+    <t>Ajout de l'unitée (degrée °) sur l'échelle de température sur le graphique</t>
+  </si>
+  <si>
+    <t>Discussion avec le prof concernant mon projet, réorientation de la manière de faire mon projet, au lieu de demander ce que veut l'utilisateur et faire une requête API en conséquence à chaque fois pour afficher les données il faut que l'utilisateur fasse une requête, ensuite il faut aller voir dans mes fichiers CSV si j'ai les données nécessaires pour répondre à ses attentes si je ne les aient pas je vais les chercher via l'API et je les rajoute à mon CSV et finalement je projette les données via mon CSV en filtrant avec LINQ</t>
+  </si>
+  <si>
+    <t>Création UserStories et test d'acceptance</t>
+  </si>
+  <si>
+    <t>J'ai commencé à implémenter la UserStory Liste des villes, mais il n'y pas grand-chose d'interessant pour l'instant, pour la prochaine fois il faudra pouvoir 1. Afficher les villes dans une liste 2. Pouvoir sélectionner les villes de la liste 3. Pouvoir ajouter une ville à la liste via un formulaire dans le programme 4. Et finalement que chaque ville de la liste ait une fichier CSV qui se fais remplir à chaque fois qu'il manque des données par rapport aux requêtes de l'utilisateur (Il se fait remplir via des requêtes API)</t>
   </si>
 </sst>
 </file>
@@ -1100,16 +1115,16 @@
                 <c:formatCode>hh\ "h"\ mm\ "min"</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>0.10069444444444445</c:v>
+                  <c:v>0.11805555555555555</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.12847222222222221</c:v>
+                  <c:v>0.1875</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.0416666666666666E-2</c:v>
+                  <c:v>1.7361111111111112E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>8.6805555555555552E-2</c:v>
@@ -1121,7 +1136,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3.125E-2</c:v>
+                  <c:v>7.2916666666666671E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2033,8 +2048,8 @@
   <dimension ref="A1:O532"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B25" sqref="B25"/>
+      <pane ySplit="6" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2087,7 +2102,7 @@
       </c>
       <c r="C3" s="23" t="str">
         <f>INT(E4/1440)&amp;" jours "&amp;INT(MOD(E4/1440,1)*24)&amp;" heurs "&amp;INT(MOD(MOD(E4/1440,1)*24,1)*60)&amp;" minutes"</f>
-        <v>0 jours 8 heurs 35 minutes</v>
+        <v>0 jours 11 heurs 35 minutes</v>
       </c>
       <c r="D3" s="23"/>
       <c r="E3" s="3"/>
@@ -2106,11 +2121,11 @@
       </c>
       <c r="D4" s="23">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>275</v>
+        <v>455</v>
       </c>
       <c r="E4" s="41">
         <f>SUM(C4:D4)</f>
-        <v>515</v>
+        <v>695</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="7"/>
@@ -2599,87 +2614,141 @@
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" s="17">
         <f>IF(ISBLANK(B25),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B25))</f>
+        <v>38</v>
+      </c>
+      <c r="B25" s="51">
+        <v>45555</v>
+      </c>
+      <c r="C25" s="52"/>
+      <c r="D25" s="53">
+        <v>25</v>
+      </c>
+      <c r="E25" s="54" t="s">
+        <v>22</v>
+      </c>
+      <c r="F25" s="37" t="s">
+        <v>46</v>
+      </c>
+      <c r="G25" s="18"/>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A26" s="8">
+        <f>IF(ISBLANK(B26),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B26))</f>
+        <v>38</v>
+      </c>
+      <c r="B26" s="47">
+        <v>45555</v>
+      </c>
+      <c r="C26" s="48"/>
+      <c r="D26" s="49">
+        <v>55</v>
+      </c>
+      <c r="E26" s="50" t="s">
+        <v>4</v>
+      </c>
+      <c r="F26" s="37" t="s">
+        <v>47</v>
+      </c>
+      <c r="G26" s="16"/>
+    </row>
+    <row r="27" spans="1:15" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="A27" s="17">
+        <f>IF(ISBLANK(B27),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B27))</f>
+        <v>38</v>
+      </c>
+      <c r="B27" s="51">
+        <v>45555</v>
+      </c>
+      <c r="C27" s="52"/>
+      <c r="D27" s="53">
+        <v>30</v>
+      </c>
+      <c r="E27" s="54" t="s">
+        <v>22</v>
+      </c>
+      <c r="F27" s="37" t="s">
+        <v>48</v>
+      </c>
+      <c r="G27" s="18"/>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A28" s="8">
+        <f>IF(ISBLANK(B28),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B28))</f>
+        <v>38</v>
+      </c>
+      <c r="B28" s="47">
+        <v>45555</v>
+      </c>
+      <c r="C28" s="48"/>
+      <c r="D28" s="49">
+        <v>25</v>
+      </c>
+      <c r="E28" s="50" t="s">
+        <v>3</v>
+      </c>
+      <c r="F28" s="36" t="s">
+        <v>49</v>
+      </c>
+      <c r="G28" s="16"/>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A29" s="17">
+        <f>IF(ISBLANK(B29),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B29))</f>
+        <v>38</v>
+      </c>
+      <c r="B29" s="51">
+        <v>45555</v>
+      </c>
+      <c r="C29" s="52"/>
+      <c r="D29" s="53">
+        <v>10</v>
+      </c>
+      <c r="E29" s="54" t="s">
+        <v>6</v>
+      </c>
+      <c r="F29" s="36" t="s">
         <v>37</v>
       </c>
-      <c r="B25" s="51">
-        <v>45548</v>
-      </c>
-      <c r="C25" s="52"/>
-      <c r="D25" s="53"/>
-      <c r="E25" s="54"/>
-      <c r="F25" s="37"/>
-      <c r="G25" s="18"/>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A26" s="8" t="str">
-        <f>IF(ISBLANK(B26),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B26))</f>
-        <v/>
-      </c>
-      <c r="B26" s="47"/>
-      <c r="C26" s="48"/>
-      <c r="D26" s="49"/>
-      <c r="E26" s="50"/>
-      <c r="F26" s="37"/>
-      <c r="G26" s="16"/>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A27" s="17" t="str">
-        <f>IF(ISBLANK(B27),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B27))</f>
-        <v/>
-      </c>
-      <c r="B27" s="51"/>
-      <c r="C27" s="52"/>
-      <c r="D27" s="53"/>
-      <c r="E27" s="54"/>
-      <c r="F27" s="37"/>
-      <c r="G27" s="18"/>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A28" s="8" t="str">
-        <f>IF(ISBLANK(B28),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B28))</f>
-        <v/>
-      </c>
-      <c r="B28" s="47"/>
-      <c r="C28" s="48"/>
-      <c r="D28" s="49"/>
-      <c r="E28" s="50"/>
-      <c r="F28" s="36"/>
-      <c r="G28" s="16"/>
-    </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A29" s="17" t="str">
-        <f>IF(ISBLANK(B29),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B29))</f>
-        <v/>
-      </c>
-      <c r="B29" s="51"/>
-      <c r="C29" s="52"/>
-      <c r="D29" s="53"/>
-      <c r="E29" s="54"/>
-      <c r="F29" s="36"/>
       <c r="G29" s="18"/>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A30" s="8" t="str">
+    <row r="30" spans="1:15" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="A30" s="8">
         <f>IF(ISBLANK(B30),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B30))</f>
-        <v/>
-      </c>
-      <c r="B30" s="47"/>
+        <v>38</v>
+      </c>
+      <c r="B30" s="47">
+        <v>45555</v>
+      </c>
       <c r="C30" s="48"/>
-      <c r="D30" s="49"/>
-      <c r="E30" s="50"/>
-      <c r="F30" s="37"/>
+      <c r="D30" s="49">
+        <v>30</v>
+      </c>
+      <c r="E30" s="50" t="s">
+        <v>4</v>
+      </c>
+      <c r="F30" s="37" t="s">
+        <v>50</v>
+      </c>
       <c r="G30" s="16"/>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A31" s="17" t="str">
+      <c r="A31" s="17">
         <f>IF(ISBLANK(B31),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B31))</f>
-        <v/>
-      </c>
-      <c r="B31" s="51"/>
+        <v>38</v>
+      </c>
+      <c r="B31" s="51">
+        <v>45555</v>
+      </c>
       <c r="C31" s="52"/>
-      <c r="D31" s="53"/>
-      <c r="E31" s="54"/>
-      <c r="F31" s="36"/>
+      <c r="D31" s="53">
+        <v>5</v>
+      </c>
+      <c r="E31" s="54" t="s">
+        <v>22</v>
+      </c>
+      <c r="F31" s="36" t="s">
+        <v>44</v>
+      </c>
       <c r="G31" s="18"/>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
@@ -8785,7 +8854,7 @@
       </c>
       <c r="B4">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C4,'Journal de travail'!$D$7:$D$532)</f>
-        <v>85</v>
+        <v>110</v>
       </c>
       <c r="C4" s="26" t="str">
         <f>'Journal de travail'!M8</f>
@@ -8793,7 +8862,7 @@
       </c>
       <c r="D4" s="34">
         <f>(A4+B4)/1440</f>
-        <v>0.10069444444444445</v>
+        <v>0.11805555555555555</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -8803,7 +8872,7 @@
       </c>
       <c r="B5">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C5,'Journal de travail'!$D$7:$D$532)</f>
-        <v>65</v>
+        <v>150</v>
       </c>
       <c r="C5" s="42" t="str">
         <f>'Journal de travail'!M9</f>
@@ -8811,7 +8880,7 @@
       </c>
       <c r="D5" s="34">
         <f t="shared" ref="D5:D11" si="0">(A5+B5)/1440</f>
-        <v>0.12847222222222221</v>
+        <v>0.1875</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -8839,7 +8908,7 @@
       </c>
       <c r="B7">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C7,'Journal de travail'!$D$7:$D$532)</f>
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="C7" s="28" t="str">
         <f>'Journal de travail'!M11</f>
@@ -8847,7 +8916,7 @@
       </c>
       <c r="D7" s="34">
         <f t="shared" si="0"/>
-        <v>1.0416666666666666E-2</v>
+        <v>1.7361111111111112E-2</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -8903,7 +8972,7 @@
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B11">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C11,'Journal de travail'!$D$7:$D$532)</f>
-        <v>45</v>
+        <v>105</v>
       </c>
       <c r="C11" s="40" t="str">
         <f>'Journal de travail'!M15</f>
@@ -8911,7 +8980,7 @@
       </c>
       <c r="D11" s="34">
         <f t="shared" si="0"/>
-        <v>3.125E-2</v>
+        <v>7.2916666666666671E-2</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
@@ -8920,7 +8989,7 @@
       </c>
       <c r="D12" s="35">
         <f>SUM(D4:D11)</f>
-        <v>0.35763888888888884</v>
+        <v>0.4826388888888889</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -8934,6 +9003,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D4F20F00DBE2EE49BE9523363A2DF18B" ma:contentTypeVersion="13" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="313dbdbec26224d1c2bb7e3c488b2a4e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="99ffe1f3-7857-457f-add0-5bdef636f38d" xmlns:ns3="be0d3259-a7ce-4623-88ec-81594dfcbc1c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4739345e3d2c6be79c5ae1a54d02a4a7" ns2:_="" ns3:_="">
     <xsd:import namespace="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
@@ -9156,7 +9234,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
@@ -9167,16 +9245,15 @@
 </p:properties>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F2FB702A-DCBD-43A8-A34C-6000FD8861AD}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9195,7 +9272,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -9210,12 +9287,4 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
chore: (jnvtrl) update jnvtrl
</commit_message>
<xml_diff>
--- a/Doc/JNTRVL-PlotThatLine-MaresJulien.xlsx
+++ b/Doc/JNTRVL-PlotThatLine-MaresJulien.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\px50vpm\Documents\GitHub\Plot-that-line\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF329CE8-1195-4097-8EB7-F8962B619A38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6B7BA3B-8E0E-4A29-B4E5-BACF639FFAD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="Mvap2W10CJFFJsnvkGXSiMLvpngxTMJbJsIKFe7Hzjn0XDcmjGuvBC2FjUCZ/hpRpUhUrG1T4kBlDAIo3yqmSQ==" workbookSaltValue="KXjgXOcsUZI/j7UgPKltzw==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="61">
   <si>
     <t>Journal de travail</t>
   </si>
@@ -213,6 +213,21 @@
   </si>
   <si>
     <t>J'ai crée un formulaire ou on peut ajouter une ville en donnant des informations formulaire "addCity"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Discussion avec le prof   </t>
+  </si>
+  <si>
+    <t>J'ai modifié mon code afin de pouvoir : retrouver les villes selectionné dans la checkedlist dans la liste des villes contenant des objets city et de recréer une liste avec seulement les élements selectionné dans la liste ensuite je peux afficher sur le graph les données comme avant mais de toutes les villes selectionné</t>
+  </si>
+  <si>
+    <t>Beaucoup de probleme avc gitignore j'ai supprimé un projet visual studio que j'avais crée au début sauf que je n'avais pas encore de gitignore donc ca m'a fait un commits avec des centaines de fichiers etc.. Finalement jai réussi à le supprimer même si j'ai du avoir 1 commit par atomique dutout maintenant je pense savoir pourquoi il reste qq fichier qui sont versionner alors que je le veux pas, c'est parce que ils ont commencé a etre versionné avant quil y ait le gitignore et le sont donc toujours, il faudrait que je trouve le temps de régler ce probleme</t>
+  </si>
+  <si>
+    <t>Refactorisation du code (chatgpt m'a aidé pas mal)</t>
+  </si>
+  <si>
+    <t>Ajout dans la design  pour les fonctionnalitées utilisateurs (datepicker) (button recherche) etc..</t>
   </si>
 </sst>
 </file>
@@ -1133,13 +1148,13 @@
                   <c:v>0.11805555555555555</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.30555555555555558</c:v>
+                  <c:v>0.38541666666666669</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.7361111111111112E-2</c:v>
+                  <c:v>2.4305555555555556E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>8.6805555555555552E-2</c:v>
@@ -1151,7 +1166,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>7.9861111111111105E-2</c:v>
+                  <c:v>0.11805555555555555</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2064,7 +2079,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D36" sqref="D36"/>
+      <selection pane="bottomLeft" activeCell="F44" sqref="F44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2117,7 +2132,7 @@
       </c>
       <c r="C3" s="23" t="str">
         <f>INT(E4/1440)&amp;" jours "&amp;INT(MOD(E4/1440,1)*24)&amp;" heurs "&amp;INT(MOD(MOD(E4/1440,1)*24,1)*60)&amp;" minutes"</f>
-        <v>0 jours 14 heurs 34 minutes</v>
+        <v>0 jours 17 heurs 34 minutes</v>
       </c>
       <c r="D3" s="23"/>
       <c r="E3" s="3"/>
@@ -2132,15 +2147,15 @@
       <c r="B4" s="5"/>
       <c r="C4" s="23">
         <f>SUBTOTAL(9,$C$7:$C$531)*60</f>
-        <v>360</v>
+        <v>420</v>
       </c>
       <c r="D4" s="23">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>515</v>
+        <v>635</v>
       </c>
       <c r="E4" s="41">
         <f>SUM(C4:D4)</f>
-        <v>875</v>
+        <v>1055</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="7"/>
@@ -2849,11 +2864,13 @@
       <c r="G35" s="18"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="8" t="str">
+      <c r="A36" s="8">
         <f>IF(ISBLANK(B36),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B36))</f>
-        <v/>
-      </c>
-      <c r="B36" s="47"/>
+        <v>39</v>
+      </c>
+      <c r="B36" s="47">
+        <v>45562</v>
+      </c>
       <c r="C36" s="48">
         <v>1</v>
       </c>
@@ -2869,87 +2886,145 @@
       <c r="G36" s="16"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="17" t="str">
+      <c r="A37" s="17">
         <f>IF(ISBLANK(B37),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B37))</f>
-        <v/>
-      </c>
-      <c r="B37" s="51"/>
+        <v>40</v>
+      </c>
+      <c r="B37" s="51">
+        <v>45569</v>
+      </c>
       <c r="C37" s="52"/>
-      <c r="D37" s="53"/>
-      <c r="E37" s="54"/>
-      <c r="F37" s="36"/>
+      <c r="D37" s="53">
+        <v>20</v>
+      </c>
+      <c r="E37" s="54" t="s">
+        <v>22</v>
+      </c>
+      <c r="F37" s="36" t="s">
+        <v>56</v>
+      </c>
       <c r="G37" s="18"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" s="8" t="str">
+      <c r="A38" s="8">
         <f>IF(ISBLANK(B38),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B38))</f>
-        <v/>
-      </c>
-      <c r="B38" s="47"/>
+        <v>40</v>
+      </c>
+      <c r="B38" s="47">
+        <v>45569</v>
+      </c>
       <c r="C38" s="48"/>
-      <c r="D38" s="49"/>
-      <c r="E38" s="50"/>
-      <c r="F38" s="36"/>
+      <c r="D38" s="49">
+        <v>5</v>
+      </c>
+      <c r="E38" s="50" t="s">
+        <v>22</v>
+      </c>
+      <c r="F38" s="36" t="s">
+        <v>44</v>
+      </c>
       <c r="G38" s="16"/>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" s="17" t="str">
+      <c r="A39" s="17">
         <f>IF(ISBLANK(B39),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B39))</f>
-        <v/>
-      </c>
-      <c r="B39" s="51"/>
-      <c r="C39" s="52"/>
-      <c r="D39" s="53"/>
-      <c r="E39" s="54"/>
-      <c r="F39" s="36"/>
+        <v>40</v>
+      </c>
+      <c r="B39" s="51">
+        <v>45569</v>
+      </c>
+      <c r="C39" s="52">
+        <v>1</v>
+      </c>
+      <c r="D39" s="53">
+        <v>0</v>
+      </c>
+      <c r="E39" s="54" t="s">
+        <v>4</v>
+      </c>
+      <c r="F39" s="36" t="s">
+        <v>57</v>
+      </c>
       <c r="G39" s="18"/>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" s="8" t="str">
+      <c r="A40" s="8">
         <f>IF(ISBLANK(B40),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B40))</f>
-        <v/>
-      </c>
-      <c r="B40" s="47"/>
+        <v>40</v>
+      </c>
+      <c r="B40" s="47">
+        <v>45569</v>
+      </c>
       <c r="C40" s="48"/>
-      <c r="D40" s="49"/>
-      <c r="E40" s="50"/>
-      <c r="F40" s="36"/>
+      <c r="D40" s="49">
+        <v>30</v>
+      </c>
+      <c r="E40" s="50" t="s">
+        <v>22</v>
+      </c>
+      <c r="F40" s="36" t="s">
+        <v>58</v>
+      </c>
       <c r="G40" s="16"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" s="17" t="str">
+      <c r="A41" s="17">
         <f>IF(ISBLANK(B41),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B41))</f>
-        <v/>
-      </c>
-      <c r="B41" s="51"/>
+        <v>40</v>
+      </c>
+      <c r="B41" s="51">
+        <v>45569</v>
+      </c>
       <c r="C41" s="52"/>
-      <c r="D41" s="53"/>
-      <c r="E41" s="54"/>
-      <c r="F41" s="36"/>
+      <c r="D41" s="53">
+        <v>20</v>
+      </c>
+      <c r="E41" s="54" t="s">
+        <v>4</v>
+      </c>
+      <c r="F41" s="36" t="s">
+        <v>59</v>
+      </c>
       <c r="G41" s="18"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" s="8" t="str">
+      <c r="A42" s="8">
         <f>IF(ISBLANK(B42),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B42))</f>
-        <v/>
-      </c>
-      <c r="B42" s="47"/>
+        <v>40</v>
+      </c>
+      <c r="B42" s="47">
+        <v>45569</v>
+      </c>
       <c r="C42" s="48"/>
-      <c r="D42" s="49"/>
-      <c r="E42" s="50"/>
-      <c r="F42" s="36"/>
+      <c r="D42" s="49">
+        <v>10</v>
+      </c>
+      <c r="E42" s="50" t="s">
+        <v>6</v>
+      </c>
+      <c r="F42" s="36" t="s">
+        <v>37</v>
+      </c>
       <c r="G42" s="16"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" s="17" t="str">
+      <c r="A43" s="17">
         <f>IF(ISBLANK(B43),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B43))</f>
-        <v/>
-      </c>
-      <c r="B43" s="51"/>
+        <v>40</v>
+      </c>
+      <c r="B43" s="51">
+        <v>45569</v>
+      </c>
       <c r="C43" s="52"/>
-      <c r="D43" s="53"/>
-      <c r="E43" s="54"/>
-      <c r="F43" s="36"/>
+      <c r="D43" s="53">
+        <v>35</v>
+      </c>
+      <c r="E43" s="54" t="s">
+        <v>4</v>
+      </c>
+      <c r="F43" s="36" t="s">
+        <v>60</v>
+      </c>
       <c r="G43" s="18"/>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
@@ -8925,11 +9000,11 @@
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C5,'Journal de travail'!$C$7:$C$532)*60</f>
-        <v>240</v>
+        <v>300</v>
       </c>
       <c r="B5">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C5,'Journal de travail'!$D$7:$D$532)</f>
-        <v>200</v>
+        <v>255</v>
       </c>
       <c r="C5" s="42" t="str">
         <f>'Journal de travail'!M9</f>
@@ -8937,7 +9012,7 @@
       </c>
       <c r="D5" s="34">
         <f t="shared" ref="D5:D11" si="0">(A5+B5)/1440</f>
-        <v>0.30555555555555558</v>
+        <v>0.38541666666666669</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -8965,7 +9040,7 @@
       </c>
       <c r="B7">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C7,'Journal de travail'!$D$7:$D$532)</f>
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="C7" s="28" t="str">
         <f>'Journal de travail'!M11</f>
@@ -8973,7 +9048,7 @@
       </c>
       <c r="D7" s="34">
         <f t="shared" si="0"/>
-        <v>1.7361111111111112E-2</v>
+        <v>2.4305555555555556E-2</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -9029,7 +9104,7 @@
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B11">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C11,'Journal de travail'!$D$7:$D$532)</f>
-        <v>115</v>
+        <v>170</v>
       </c>
       <c r="C11" s="40" t="str">
         <f>'Journal de travail'!M15</f>
@@ -9037,7 +9112,7 @@
       </c>
       <c r="D11" s="34">
         <f t="shared" si="0"/>
-        <v>7.9861111111111105E-2</v>
+        <v>0.11805555555555555</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
@@ -9046,7 +9121,7 @@
       </c>
       <c r="D12" s="35">
         <f>SUM(D4:D11)</f>
-        <v>0.60763888888888884</v>
+        <v>0.73263888888888895</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -9069,17 +9144,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="99ffe1f3-7857-457f-add0-5bdef636f38d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D4F20F00DBE2EE49BE9523363A2DF18B" ma:contentTypeVersion="13" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="313dbdbec26224d1c2bb7e3c488b2a4e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="99ffe1f3-7857-457f-add0-5bdef636f38d" xmlns:ns3="be0d3259-a7ce-4623-88ec-81594dfcbc1c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4739345e3d2c6be79c5ae1a54d02a4a7" ns2:_="" ns3:_="">
     <xsd:import namespace="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
@@ -9302,6 +9366,17 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="99ffe1f3-7857-457f-add0-5bdef636f38d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
   <ds:schemaRefs>
@@ -9311,23 +9386,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F2FB702A-DCBD-43A8-A34C-6000FD8861AD}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9344,4 +9402,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Chore: (nvtrl) Update jnvtrl
</commit_message>
<xml_diff>
--- a/Doc/JNTRVL-PlotThatLine-MaresJulien.xlsx
+++ b/Doc/JNTRVL-PlotThatLine-MaresJulien.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\px50vpm\Documents\GitHub\Plot-that-line\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6B7BA3B-8E0E-4A29-B4E5-BACF639FFAD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD304F8C-43C8-4187-9BD3-AF45A47926FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="Mvap2W10CJFFJsnvkGXSiMLvpngxTMJbJsIKFe7Hzjn0XDcmjGuvBC2FjUCZ/hpRpUhUrG1T4kBlDAIo3yqmSQ==" workbookSaltValue="KXjgXOcsUZI/j7UgPKltzw==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="66">
   <si>
     <t>Journal de travail</t>
   </si>
@@ -228,6 +228,21 @@
   </si>
   <si>
     <t>Ajout dans la design  pour les fonctionnalitées utilisateurs (datepicker) (button recherche) etc..</t>
+  </si>
+  <si>
+    <t>Creation méthode pour aller voir les fichiers dans un dossier, les lire, créer un object pour chacun d'eux (City) en faisant en sorte qu'il ne prenne pas les données météos</t>
+  </si>
+  <si>
+    <t>Le prof ns parle de plantUML et icetools</t>
+  </si>
+  <si>
+    <t>Il y a un probleme, quand je crée un json pour les objets city il n'y a pas les data meteos, j'ai essayé de le régler mais pas réussi, à faire la prochaine fois</t>
+  </si>
+  <si>
+    <t>Création de user story et de tests dacceptance</t>
+  </si>
+  <si>
+    <t>refactorisation du code (button inutile, création de méthode pour certaines choses etc..)</t>
   </si>
 </sst>
 </file>
@@ -1145,16 +1160,16 @@
                 <c:formatCode>hh\ "h"\ mm\ "min"</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>0.11805555555555555</c:v>
+                  <c:v>0.1388888888888889</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.38541666666666669</c:v>
+                  <c:v>0.47569444444444442</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.4305555555555556E-2</c:v>
+                  <c:v>3.4722222222222224E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>8.6805555555555552E-2</c:v>
@@ -1166,7 +1181,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.11805555555555555</c:v>
+                  <c:v>0.1423611111111111</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2078,8 +2093,8 @@
   <dimension ref="A1:O532"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F44" sqref="F44"/>
+      <pane ySplit="6" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F51" sqref="F51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2132,7 +2147,7 @@
       </c>
       <c r="C3" s="23" t="str">
         <f>INT(E4/1440)&amp;" jours "&amp;INT(MOD(E4/1440,1)*24)&amp;" heurs "&amp;INT(MOD(MOD(E4/1440,1)*24,1)*60)&amp;" minutes"</f>
-        <v>0 jours 17 heurs 34 minutes</v>
+        <v>0 jours 21 heurs 4 minutes</v>
       </c>
       <c r="D3" s="23"/>
       <c r="E3" s="3"/>
@@ -2151,11 +2166,11 @@
       </c>
       <c r="D4" s="23">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>635</v>
+        <v>845</v>
       </c>
       <c r="E4" s="41">
         <f>SUM(C4:D4)</f>
-        <v>1055</v>
+        <v>1265</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="7"/>
@@ -3028,87 +3043,143 @@
       <c r="G43" s="18"/>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" s="8" t="str">
+      <c r="A44" s="8">
         <f>IF(ISBLANK(B44),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B44))</f>
-        <v/>
-      </c>
-      <c r="B44" s="47"/>
+        <v>41</v>
+      </c>
+      <c r="B44" s="47">
+        <v>45576</v>
+      </c>
       <c r="C44" s="48"/>
-      <c r="D44" s="49"/>
-      <c r="E44" s="50"/>
-      <c r="F44" s="36"/>
+      <c r="D44" s="49">
+        <v>45</v>
+      </c>
+      <c r="E44" s="50" t="s">
+        <v>4</v>
+      </c>
+      <c r="F44" s="36" t="s">
+        <v>61</v>
+      </c>
       <c r="G44" s="16"/>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" s="17" t="str">
+      <c r="A45" s="17">
         <f>IF(ISBLANK(B45),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B45))</f>
-        <v/>
-      </c>
-      <c r="B45" s="51"/>
+        <v>41</v>
+      </c>
+      <c r="B45" s="51">
+        <v>45576</v>
+      </c>
       <c r="C45" s="52"/>
-      <c r="D45" s="53"/>
-      <c r="E45" s="54"/>
-      <c r="F45" s="36"/>
+      <c r="D45" s="53">
+        <v>30</v>
+      </c>
+      <c r="E45" s="54" t="s">
+        <v>22</v>
+      </c>
+      <c r="F45" s="36" t="s">
+        <v>62</v>
+      </c>
       <c r="G45" s="18"/>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" s="8" t="str">
+      <c r="A46" s="8">
         <f>IF(ISBLANK(B46),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B46))</f>
-        <v/>
-      </c>
-      <c r="B46" s="47"/>
+        <v>41</v>
+      </c>
+      <c r="B46" s="47">
+        <v>45576</v>
+      </c>
       <c r="C46" s="48"/>
-      <c r="D46" s="49"/>
-      <c r="E46" s="50"/>
-      <c r="F46" s="36"/>
+      <c r="D46" s="49">
+        <v>5</v>
+      </c>
+      <c r="E46" s="50" t="s">
+        <v>22</v>
+      </c>
+      <c r="F46" s="36" t="s">
+        <v>44</v>
+      </c>
       <c r="G46" s="16"/>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" s="17" t="str">
+      <c r="A47" s="17">
         <f>IF(ISBLANK(B47),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B47))</f>
-        <v/>
-      </c>
-      <c r="B47" s="51"/>
+        <v>41</v>
+      </c>
+      <c r="B47" s="51">
+        <v>45576</v>
+      </c>
       <c r="C47" s="52"/>
-      <c r="D47" s="53"/>
-      <c r="E47" s="54"/>
-      <c r="F47" s="36"/>
+      <c r="D47" s="53">
+        <v>55</v>
+      </c>
+      <c r="E47" s="54" t="s">
+        <v>4</v>
+      </c>
+      <c r="F47" s="36" t="s">
+        <v>63</v>
+      </c>
       <c r="G47" s="18"/>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A48" s="8" t="str">
+      <c r="A48" s="8">
         <f>IF(ISBLANK(B48),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B48))</f>
-        <v/>
-      </c>
-      <c r="B48" s="47"/>
+        <v>41</v>
+      </c>
+      <c r="B48" s="47">
+        <v>45576</v>
+      </c>
       <c r="C48" s="48"/>
-      <c r="D48" s="49"/>
-      <c r="E48" s="50"/>
-      <c r="F48" s="36"/>
+      <c r="D48" s="49">
+        <v>30</v>
+      </c>
+      <c r="E48" s="50" t="s">
+        <v>3</v>
+      </c>
+      <c r="F48" s="36" t="s">
+        <v>64</v>
+      </c>
       <c r="G48" s="16"/>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A49" s="17" t="str">
+      <c r="A49" s="17">
         <f>IF(ISBLANK(B49),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B49))</f>
-        <v/>
-      </c>
-      <c r="B49" s="51"/>
+        <v>41</v>
+      </c>
+      <c r="B49" s="51">
+        <v>45576</v>
+      </c>
       <c r="C49" s="52"/>
-      <c r="D49" s="53"/>
-      <c r="E49" s="54"/>
-      <c r="F49" s="36"/>
+      <c r="D49" s="53">
+        <v>15</v>
+      </c>
+      <c r="E49" s="54" t="s">
+        <v>6</v>
+      </c>
+      <c r="F49" s="36" t="s">
+        <v>37</v>
+      </c>
       <c r="G49" s="18"/>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A50" s="8" t="str">
+      <c r="A50" s="8">
         <f>IF(ISBLANK(B50),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B50))</f>
-        <v/>
-      </c>
-      <c r="B50" s="47"/>
+        <v>41</v>
+      </c>
+      <c r="B50" s="47">
+        <v>45576</v>
+      </c>
       <c r="C50" s="48"/>
-      <c r="D50" s="49"/>
-      <c r="E50" s="50"/>
-      <c r="F50" s="36"/>
+      <c r="D50" s="49">
+        <v>30</v>
+      </c>
+      <c r="E50" s="50" t="s">
+        <v>4</v>
+      </c>
+      <c r="F50" s="36" t="s">
+        <v>65</v>
+      </c>
       <c r="G50" s="16"/>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
@@ -8986,7 +9057,7 @@
       </c>
       <c r="B4">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C4,'Journal de travail'!$D$7:$D$532)</f>
-        <v>110</v>
+        <v>140</v>
       </c>
       <c r="C4" s="26" t="str">
         <f>'Journal de travail'!M8</f>
@@ -8994,7 +9065,7 @@
       </c>
       <c r="D4" s="34">
         <f>(A4+B4)/1440</f>
-        <v>0.11805555555555555</v>
+        <v>0.1388888888888889</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -9004,7 +9075,7 @@
       </c>
       <c r="B5">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C5,'Journal de travail'!$D$7:$D$532)</f>
-        <v>255</v>
+        <v>385</v>
       </c>
       <c r="C5" s="42" t="str">
         <f>'Journal de travail'!M9</f>
@@ -9012,7 +9083,7 @@
       </c>
       <c r="D5" s="34">
         <f t="shared" ref="D5:D11" si="0">(A5+B5)/1440</f>
-        <v>0.38541666666666669</v>
+        <v>0.47569444444444442</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -9040,7 +9111,7 @@
       </c>
       <c r="B7">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C7,'Journal de travail'!$D$7:$D$532)</f>
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="C7" s="28" t="str">
         <f>'Journal de travail'!M11</f>
@@ -9048,7 +9119,7 @@
       </c>
       <c r="D7" s="34">
         <f t="shared" si="0"/>
-        <v>2.4305555555555556E-2</v>
+        <v>3.4722222222222224E-2</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -9104,7 +9175,7 @@
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B11">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C11,'Journal de travail'!$D$7:$D$532)</f>
-        <v>170</v>
+        <v>205</v>
       </c>
       <c r="C11" s="40" t="str">
         <f>'Journal de travail'!M15</f>
@@ -9112,7 +9183,7 @@
       </c>
       <c r="D11" s="34">
         <f t="shared" si="0"/>
-        <v>0.11805555555555555</v>
+        <v>0.1423611111111111</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
@@ -9121,7 +9192,7 @@
       </c>
       <c r="D12" s="35">
         <f>SUM(D4:D11)</f>
-        <v>0.73263888888888895</v>
+        <v>0.8784722222222221</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -9144,6 +9215,17 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="99ffe1f3-7857-457f-add0-5bdef636f38d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D4F20F00DBE2EE49BE9523363A2DF18B" ma:contentTypeVersion="13" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="313dbdbec26224d1c2bb7e3c488b2a4e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="99ffe1f3-7857-457f-add0-5bdef636f38d" xmlns:ns3="be0d3259-a7ce-4623-88ec-81594dfcbc1c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4739345e3d2c6be79c5ae1a54d02a4a7" ns2:_="" ns3:_="">
     <xsd:import namespace="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
@@ -9366,17 +9448,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="99ffe1f3-7857-457f-add0-5bdef636f38d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
   <ds:schemaRefs>
@@ -9386,6 +9457,23 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F2FB702A-DCBD-43A8-A34C-6000FD8861AD}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9402,21 +9490,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Chore : (jnvtrl) Update journal de travail
</commit_message>
<xml_diff>
--- a/Doc/JNTRVL-PlotThatLine-MaresJulien.xlsx
+++ b/Doc/JNTRVL-PlotThatLine-MaresJulien.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\px50vpm\Documents\GitHub\Plot-that-line\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD304F8C-43C8-4187-9BD3-AF45A47926FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EC82FCA-477A-46B6-8D84-1D972FBC5FC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="Mvap2W10CJFFJsnvkGXSiMLvpngxTMJbJsIKFe7Hzjn0XDcmjGuvBC2FjUCZ/hpRpUhUrG1T4kBlDAIo3yqmSQ==" workbookSaltValue="KXjgXOcsUZI/j7UgPKltzw==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="71">
   <si>
     <t>Journal de travail</t>
   </si>
@@ -243,6 +243,21 @@
   </si>
   <si>
     <t>refactorisation du code (button inutile, création de méthode pour certaines choses etc..)</t>
+  </si>
+  <si>
+    <t>régler problèmes github, (c'est un peu long à faire mais il fallait pour tout les fichiers ou dossiers qui était versionner et quon ne voulait pas, les supprimer puis faire dans git bash git rm -r (chemin vers le dossier)</t>
+  </si>
+  <si>
+    <t>Création de user stories et de test d'acceptance</t>
+  </si>
+  <si>
+    <t>Création méthode pour récupérer les données métérologique (la partie local surtout, avec l'API c'était deja fais il y a juste eu quelque modification à faire)</t>
+  </si>
+  <si>
+    <t>méthode "StoreDataAsync) pour stocker/mettre à jour les données dans le json via les données de l'objet (remplis via l'API)</t>
+  </si>
+  <si>
+    <t>Faire en sorte que le graph soit mis à jour sans avoir à le refresh avec le bouton (si on sélectionne une nvl city par exemple ou quon change la date de début etc...)</t>
   </si>
 </sst>
 </file>
@@ -1160,10 +1175,10 @@
                 <c:formatCode>hh\ "h"\ mm\ "min"</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>0.1388888888888889</c:v>
+                  <c:v>0.19444444444444445</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.47569444444444442</c:v>
+                  <c:v>0.67013888888888884</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -1181,7 +1196,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.1423611111111111</c:v>
+                  <c:v>0.1701388888888889</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2093,8 +2108,8 @@
   <dimension ref="A1:O532"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F51" sqref="F51"/>
+      <pane ySplit="6" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F42" sqref="F42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2147,7 +2162,7 @@
       </c>
       <c r="C3" s="23" t="str">
         <f>INT(E4/1440)&amp;" jours "&amp;INT(MOD(E4/1440,1)*24)&amp;" heurs "&amp;INT(MOD(MOD(E4/1440,1)*24,1)*60)&amp;" minutes"</f>
-        <v>0 jours 21 heurs 4 minutes</v>
+        <v>1 jours 3 heurs 45 minutes</v>
       </c>
       <c r="D3" s="23"/>
       <c r="E3" s="3"/>
@@ -2162,15 +2177,15 @@
       <c r="B4" s="5"/>
       <c r="C4" s="23">
         <f>SUBTOTAL(9,$C$7:$C$531)*60</f>
-        <v>420</v>
+        <v>720</v>
       </c>
       <c r="D4" s="23">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>845</v>
+        <v>945</v>
       </c>
       <c r="E4" s="41">
         <f>SUM(C4:D4)</f>
-        <v>1265</v>
+        <v>1665</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="7"/>
@@ -3183,83 +3198,139 @@
       <c r="G50" s="16"/>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A51" s="17" t="str">
+      <c r="A51" s="17">
         <f>IF(ISBLANK(B51),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B51))</f>
-        <v/>
-      </c>
-      <c r="B51" s="51"/>
+        <v>43</v>
+      </c>
+      <c r="B51" s="51">
+        <v>45587</v>
+      </c>
       <c r="C51" s="52"/>
-      <c r="D51" s="53"/>
-      <c r="E51" s="54"/>
-      <c r="F51" s="36"/>
+      <c r="D51" s="53">
+        <v>40</v>
+      </c>
+      <c r="E51" s="54" t="s">
+        <v>22</v>
+      </c>
+      <c r="F51" s="36" t="s">
+        <v>66</v>
+      </c>
       <c r="G51" s="18"/>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A52" s="8" t="str">
+      <c r="A52" s="8">
         <f>IF(ISBLANK(B52),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B52))</f>
-        <v/>
-      </c>
-      <c r="B52" s="47"/>
-      <c r="C52" s="48"/>
-      <c r="D52" s="49"/>
-      <c r="E52" s="50"/>
-      <c r="F52" s="36"/>
+        <v>43</v>
+      </c>
+      <c r="B52" s="47">
+        <v>45587</v>
+      </c>
+      <c r="C52" s="48">
+        <v>1</v>
+      </c>
+      <c r="D52" s="49">
+        <v>20</v>
+      </c>
+      <c r="E52" s="50" t="s">
+        <v>3</v>
+      </c>
+      <c r="F52" s="36" t="s">
+        <v>67</v>
+      </c>
       <c r="G52" s="16"/>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A53" s="17" t="str">
+      <c r="A53" s="17">
         <f>IF(ISBLANK(B53),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B53))</f>
-        <v/>
-      </c>
-      <c r="B53" s="51"/>
-      <c r="C53" s="52"/>
-      <c r="D53" s="53"/>
-      <c r="E53" s="54"/>
-      <c r="F53" s="36"/>
+        <v>43</v>
+      </c>
+      <c r="B53" s="51">
+        <v>45587</v>
+      </c>
+      <c r="C53" s="52">
+        <v>2</v>
+      </c>
+      <c r="D53" s="53">
+        <v>0</v>
+      </c>
+      <c r="E53" s="54" t="s">
+        <v>4</v>
+      </c>
+      <c r="F53" s="36" t="s">
+        <v>68</v>
+      </c>
       <c r="G53" s="18"/>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A54" s="8" t="str">
+      <c r="A54" s="8">
         <f>IF(ISBLANK(B54),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B54))</f>
-        <v/>
-      </c>
-      <c r="B54" s="47"/>
-      <c r="C54" s="48"/>
-      <c r="D54" s="49"/>
-      <c r="E54" s="50"/>
-      <c r="F54" s="36"/>
+        <v>43</v>
+      </c>
+      <c r="B54" s="47">
+        <v>45588</v>
+      </c>
+      <c r="C54" s="48">
+        <v>1</v>
+      </c>
+      <c r="D54" s="49">
+        <v>10</v>
+      </c>
+      <c r="E54" s="50" t="s">
+        <v>4</v>
+      </c>
+      <c r="F54" s="36" t="s">
+        <v>69</v>
+      </c>
       <c r="G54" s="16"/>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A55" s="17" t="str">
+      <c r="A55" s="17">
         <f>IF(ISBLANK(B55),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B55))</f>
-        <v/>
-      </c>
-      <c r="B55" s="51"/>
-      <c r="C55" s="52"/>
-      <c r="D55" s="53"/>
-      <c r="E55" s="54"/>
-      <c r="F55" s="36"/>
+        <v>43</v>
+      </c>
+      <c r="B55" s="51">
+        <v>45588</v>
+      </c>
+      <c r="C55" s="52">
+        <v>1</v>
+      </c>
+      <c r="D55" s="53">
+        <v>0</v>
+      </c>
+      <c r="E55" s="54" t="s">
+        <v>4</v>
+      </c>
+      <c r="F55" s="36" t="s">
+        <v>70</v>
+      </c>
       <c r="G55" s="18"/>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A56" s="8" t="str">
+      <c r="A56" s="8">
         <f>IF(ISBLANK(B56),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B56))</f>
-        <v/>
-      </c>
-      <c r="B56" s="47"/>
+        <v>43</v>
+      </c>
+      <c r="B56" s="47">
+        <v>45588</v>
+      </c>
       <c r="C56" s="48"/>
-      <c r="D56" s="49"/>
-      <c r="E56" s="50"/>
+      <c r="D56" s="49">
+        <v>30</v>
+      </c>
+      <c r="E56" s="50" t="s">
+        <v>4</v>
+      </c>
       <c r="F56" s="16"/>
       <c r="G56" s="16"/>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A57" s="17" t="str">
+      <c r="A57" s="17">
         <f>IF(ISBLANK(B57),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B57))</f>
-        <v/>
-      </c>
-      <c r="B57" s="51"/>
+        <v>43</v>
+      </c>
+      <c r="B57" s="51">
+        <v>45589</v>
+      </c>
       <c r="C57" s="52"/>
       <c r="D57" s="53"/>
       <c r="E57" s="54"/>
@@ -3267,11 +3338,13 @@
       <c r="G57" s="18"/>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A58" s="8" t="str">
+      <c r="A58" s="8">
         <f>IF(ISBLANK(B58),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B58))</f>
-        <v/>
-      </c>
-      <c r="B58" s="47"/>
+        <v>43</v>
+      </c>
+      <c r="B58" s="47">
+        <v>45589</v>
+      </c>
       <c r="C58" s="48"/>
       <c r="D58" s="49"/>
       <c r="E58" s="50"/>
@@ -9053,11 +9126,11 @@
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C4,'Journal de travail'!$C$7:$C$532)*60</f>
-        <v>60</v>
+        <v>120</v>
       </c>
       <c r="B4">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C4,'Journal de travail'!$D$7:$D$532)</f>
-        <v>140</v>
+        <v>160</v>
       </c>
       <c r="C4" s="26" t="str">
         <f>'Journal de travail'!M8</f>
@@ -9065,17 +9138,17 @@
       </c>
       <c r="D4" s="34">
         <f>(A4+B4)/1440</f>
-        <v>0.1388888888888889</v>
+        <v>0.19444444444444445</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C5,'Journal de travail'!$C$7:$C$532)*60</f>
-        <v>300</v>
+        <v>540</v>
       </c>
       <c r="B5">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C5,'Journal de travail'!$D$7:$D$532)</f>
-        <v>385</v>
+        <v>425</v>
       </c>
       <c r="C5" s="42" t="str">
         <f>'Journal de travail'!M9</f>
@@ -9083,7 +9156,7 @@
       </c>
       <c r="D5" s="34">
         <f t="shared" ref="D5:D11" si="0">(A5+B5)/1440</f>
-        <v>0.47569444444444442</v>
+        <v>0.67013888888888884</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -9175,7 +9248,7 @@
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B11">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C11,'Journal de travail'!$D$7:$D$532)</f>
-        <v>205</v>
+        <v>245</v>
       </c>
       <c r="C11" s="40" t="str">
         <f>'Journal de travail'!M15</f>
@@ -9183,7 +9256,7 @@
       </c>
       <c r="D11" s="34">
         <f t="shared" si="0"/>
-        <v>0.1423611111111111</v>
+        <v>0.1701388888888889</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
@@ -9192,7 +9265,7 @@
       </c>
       <c r="D12" s="35">
         <f>SUM(D4:D11)</f>
-        <v>0.8784722222222221</v>
+        <v>1.15625</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -9459,16 +9532,16 @@
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
     <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Chore : (jnvtrl) update jnvtrl
</commit_message>
<xml_diff>
--- a/Doc/JNTRVL-PlotThatLine-MaresJulien.xlsx
+++ b/Doc/JNTRVL-PlotThatLine-MaresJulien.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\px50vpm\Documents\GitHub\Plot-that-line\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EC82FCA-477A-46B6-8D84-1D972FBC5FC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{289A512A-C3E9-46A1-9C5F-824D37D96713}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="Mvap2W10CJFFJsnvkGXSiMLvpngxTMJbJsIKFe7Hzjn0XDcmjGuvBC2FjUCZ/hpRpUhUrG1T4kBlDAIo3yqmSQ==" workbookSaltValue="KXjgXOcsUZI/j7UgPKltzw==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="74">
   <si>
     <t>Journal de travail</t>
   </si>
@@ -258,6 +258,15 @@
   </si>
   <si>
     <t>Faire en sorte que le graph soit mis à jour sans avoir à le refresh avec le bouton (si on sélectionne une nvl city par exemple ou quon change la date de début etc...)</t>
+  </si>
+  <si>
+    <t>refactorisation/fix du code, par exemple les entrées utilisateurs doivent être controllé (latitude longitude etc)</t>
+  </si>
+  <si>
+    <t>Icetools</t>
+  </si>
+  <si>
+    <t>Refactorisation du code pour plusieurs raison, avant cela prennait les données meteo puis les stockait dans le fichiers json (seulementl e laps de temps selectionné) sauf qu'il y avait plusieurs raison de changer ça 1. à l'avenir les données récents vont sûrement être utilisé donc c'est une bonne chose de déjà les avoirs. 2. Le code est fais de manière à ce que si la date de début et de fin entrée par l'utilisateur est contenu dans le fichier local alors la méthode de récupération des données local se fais, le probleme c'est que si on a dans le json les données du 2mai au 6mai et du 15mai au 20mai, si l'utilisateur veut les données du 3mai au 19mai alors le programme va pensé que le fichier json contient les données puisqu'il contient les dates de fin et de début mais enft celle du milieu n'ont jamais été demandé. C'est pour cela que cette refactorisation fais en sorte de prendre les données de la date de début jusqu'à la date d'aujourd'hui (-3jours car l'API n'est pas mis à jour le jour même). Et c'est ensuite pendant l'affichage qu'on va trier les données qu'on veut afficher parmis toutes celles qu'on possèdes grâce à la programmation fonctionnel (LINQ)</t>
   </si>
 </sst>
 </file>
@@ -1178,7 +1187,7 @@
                   <c:v>0.19444444444444445</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.67013888888888884</c:v>
+                  <c:v>0.73958333333333337</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -2109,7 +2118,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F42" sqref="F42"/>
+      <selection pane="bottomLeft" activeCell="C59" sqref="C59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2162,7 +2171,7 @@
       </c>
       <c r="C3" s="23" t="str">
         <f>INT(E4/1440)&amp;" jours "&amp;INT(MOD(E4/1440,1)*24)&amp;" heurs "&amp;INT(MOD(MOD(E4/1440,1)*24,1)*60)&amp;" minutes"</f>
-        <v>1 jours 3 heurs 45 minutes</v>
+        <v>1 jours 5 heurs 25 minutes</v>
       </c>
       <c r="D3" s="23"/>
       <c r="E3" s="3"/>
@@ -2177,15 +2186,15 @@
       <c r="B4" s="5"/>
       <c r="C4" s="23">
         <f>SUBTOTAL(9,$C$7:$C$531)*60</f>
-        <v>720</v>
+        <v>780</v>
       </c>
       <c r="D4" s="23">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>945</v>
+        <v>985</v>
       </c>
       <c r="E4" s="41">
         <f>SUM(C4:D4)</f>
-        <v>1665</v>
+        <v>1765</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="7"/>
@@ -3320,7 +3329,9 @@
       <c r="E56" s="50" t="s">
         <v>4</v>
       </c>
-      <c r="F56" s="16"/>
+      <c r="F56" t="s">
+        <v>71</v>
+      </c>
       <c r="G56" s="16"/>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
@@ -3332,9 +3343,15 @@
         <v>45589</v>
       </c>
       <c r="C57" s="52"/>
-      <c r="D57" s="53"/>
-      <c r="E57" s="54"/>
-      <c r="F57" s="18"/>
+      <c r="D57" s="53">
+        <v>30</v>
+      </c>
+      <c r="E57" s="54" t="s">
+        <v>4</v>
+      </c>
+      <c r="F57" t="s">
+        <v>72</v>
+      </c>
       <c r="G57" s="18"/>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
@@ -3345,10 +3362,18 @@
       <c r="B58" s="47">
         <v>45589</v>
       </c>
-      <c r="C58" s="48"/>
-      <c r="D58" s="49"/>
-      <c r="E58" s="50"/>
-      <c r="F58" s="16"/>
+      <c r="C58" s="48">
+        <v>1</v>
+      </c>
+      <c r="D58" s="49">
+        <v>10</v>
+      </c>
+      <c r="E58" s="50" t="s">
+        <v>4</v>
+      </c>
+      <c r="F58" t="s">
+        <v>73</v>
+      </c>
       <c r="G58" s="16"/>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
@@ -9042,7 +9067,7 @@
       <c r="G532" s="16"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="WocEVrSnlrnipfCRKWfJOWvVHhUwliA4sl7OFZQcnsclg1+/2zTGJR+vWYrrc9RHa1JiIfS2mDWF3//I8pwZ9g==" saltValue="/43tQAugN0SUcpU1aj1cvg==" spinCount="100000" sheet="1" insertHyperlinks="0" sort="0" autoFilter="0"/>
+  <sheetProtection insertHyperlinks="0" sort="0" autoFilter="0"/>
   <mergeCells count="2">
     <mergeCell ref="C2:E2"/>
     <mergeCell ref="C5:D5"/>
@@ -9144,11 +9169,11 @@
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C5,'Journal de travail'!$C$7:$C$532)*60</f>
-        <v>540</v>
+        <v>600</v>
       </c>
       <c r="B5">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C5,'Journal de travail'!$D$7:$D$532)</f>
-        <v>425</v>
+        <v>465</v>
       </c>
       <c r="C5" s="42" t="str">
         <f>'Journal de travail'!M9</f>
@@ -9156,7 +9181,7 @@
       </c>
       <c r="D5" s="34">
         <f t="shared" ref="D5:D11" si="0">(A5+B5)/1440</f>
-        <v>0.67013888888888884</v>
+        <v>0.73958333333333337</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -9265,14 +9290,14 @@
       </c>
       <c r="D12" s="35">
         <f>SUM(D4:D11)</f>
-        <v>1.15625</v>
+        <v>1.2256944444444444</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D14" s="39"/>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1" selectLockedCells="1" selectUnlockedCells="1"/>
+  <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -9288,17 +9313,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="99ffe1f3-7857-457f-add0-5bdef636f38d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D4F20F00DBE2EE49BE9523363A2DF18B" ma:contentTypeVersion="13" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="313dbdbec26224d1c2bb7e3c488b2a4e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="99ffe1f3-7857-457f-add0-5bdef636f38d" xmlns:ns3="be0d3259-a7ce-4623-88ec-81594dfcbc1c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4739345e3d2c6be79c5ae1a54d02a4a7" ns2:_="" ns3:_="">
     <xsd:import namespace="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
@@ -9521,6 +9535,17 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="99ffe1f3-7857-457f-add0-5bdef636f38d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
   <ds:schemaRefs>
@@ -9530,23 +9555,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
-    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F2FB702A-DCBD-43A8-A34C-6000FD8861AD}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9563,4 +9571,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>